<commit_message>
Lots of annotation to explain reasoning Applied functions for imputing missing means and sds
</commit_message>
<xml_diff>
--- a/Working_Dataset_Medication.xlsx
+++ b/Working_Dataset_Medication.xlsx
@@ -558,7 +558,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -587,6 +587,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -667,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -749,6 +755,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -3784,8 +3793,8 @@
       <c r="U23" s="6">
         <v>-22.58</v>
       </c>
-      <c r="V23" s="6">
-        <v>1.47</v>
+      <c r="V23" s="21">
+        <v>14.77</v>
       </c>
       <c r="W23" s="6">
         <v>101.0</v>
@@ -3793,8 +3802,8 @@
       <c r="X23" s="6">
         <v>-23.38</v>
       </c>
-      <c r="Y23" s="6">
-        <v>1.6</v>
+      <c r="Y23" s="21">
+        <v>16.0</v>
       </c>
       <c r="Z23" s="9">
         <v>100.0</v>
@@ -5073,8 +5082,8 @@
       <c r="T33" s="14">
         <v>117.0</v>
       </c>
-      <c r="U33" s="11">
-        <v>22.6</v>
+      <c r="U33" s="29">
+        <v>-22.6</v>
       </c>
       <c r="V33" s="11" t="s">
         <v>51</v>
@@ -5098,7 +5107,7 @@
       <c r="AD33" s="19">
         <v>0.61</v>
       </c>
-      <c r="AF33" s="29"/>
+      <c r="AF33" s="30"/>
       <c r="AG33" s="20">
         <v>0.6</v>
       </c>
@@ -6150,7 +6159,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="31" t="s">
         <v>129</v>
       </c>
       <c r="B42" s="11">
@@ -7719,8 +7728,8 @@
       <c r="AC54" s="16"/>
       <c r="AD54" s="16"/>
       <c r="AE54" s="16"/>
-      <c r="AF54" s="29"/>
-      <c r="AG54" s="29"/>
+      <c r="AF54" s="30"/>
+      <c r="AG54" s="30"/>
       <c r="AH54" s="11" t="s">
         <v>53</v>
       </c>
@@ -8432,8 +8441,8 @@
       <c r="U60" s="6">
         <v>-16.5</v>
       </c>
-      <c r="V60" s="6">
-        <v>2.45</v>
+      <c r="V60" s="21">
+        <v>13.19</v>
       </c>
       <c r="W60" s="6">
         <v>29.0</v>
@@ -8441,8 +8450,8 @@
       <c r="X60" s="6">
         <v>-11.9</v>
       </c>
-      <c r="Y60" s="6">
-        <v>2.54</v>
+      <c r="Y60" s="21">
+        <v>13.2</v>
       </c>
       <c r="Z60" s="9">
         <v>27.0</v>
@@ -9038,8 +9047,8 @@
       <c r="N65" s="9">
         <v>187.0</v>
       </c>
-      <c r="O65" s="31"/>
-      <c r="P65" s="31"/>
+      <c r="O65" s="32"/>
+      <c r="P65" s="32"/>
       <c r="Q65" s="24">
         <v>185.0</v>
       </c>
@@ -9295,10 +9304,10 @@
       <c r="N67" s="9">
         <v>85.0</v>
       </c>
-      <c r="O67" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="P67" s="33" t="s">
+      <c r="O67" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="P67" s="34" t="s">
         <v>51</v>
       </c>
       <c r="Q67" s="24">
@@ -9313,22 +9322,22 @@
       <c r="T67" s="9">
         <v>85.0</v>
       </c>
-      <c r="U67" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="V67" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="W67" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="X67" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y67" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z67" s="35" t="s">
+      <c r="U67" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="V67" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="W67" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="X67" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y67" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z67" s="36" t="s">
         <v>51</v>
       </c>
       <c r="AA67" s="6" t="s">
@@ -18303,7 +18312,7 @@
       <c r="Q1018" s="22"/>
       <c r="T1018" s="22"/>
       <c r="Z1018" s="22"/>
-      <c r="AF1018" s="29"/>
+      <c r="AF1018" s="30"/>
       <c r="AG1018" s="22"/>
     </row>
   </sheetData>

</xml_diff>